<commit_message>
refactor all current codes, move init code to class Initiator.py
</commit_message>
<xml_diff>
--- a/Backlog/Backlog.xlsx
+++ b/Backlog/Backlog.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangpengfei/project/Semantic_Checking_Tool_Py/Backlog/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22256" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GCS requirements" sheetId="1" r:id="rId1"/>
     <sheet name="FW requirements" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Requirements</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,12 +221,16 @@
     <t>GCS checker</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Wyatt Wang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -574,16 +586,16 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.90625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.6328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40.299999999999997">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -600,7 +612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="228.4">
+    <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -608,7 +620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.9">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -616,7 +628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26.9">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="255.25">
+    <row r="5" spans="1:5" ht="285" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -632,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="40.299999999999997">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -651,19 +663,19 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="16.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.90625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="4"/>
+    <col min="1" max="2" width="16.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="53.75">
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -683,7 +695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="40.299999999999997">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -693,8 +705,11 @@
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.9">
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -704,8 +719,11 @@
       <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="94.05">
+      <c r="F3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -715,8 +733,11 @@
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="26.9">
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -727,7 +748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.9">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -738,7 +759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="67.2">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -749,7 +770,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26.9">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -760,7 +781,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>